<commit_message>
added checking of prerequisites and antirequisites
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A7729C-0EF6-454C-8133-21ECE77B3FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC1F0AE-7C71-C147-BEAD-70C6BD12C2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BA51B351-0636-AB4E-9862-84BEC7942AF0}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="304">
-  <si>
-    <t>Module Code</t>
-  </si>
-  <si>
-    <t>Module Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="300">
   <si>
     <t>Year</t>
   </si>
@@ -53,9 +47,6 @@
     <t>Timetable</t>
   </si>
   <si>
-    <t>Alternate Years</t>
-  </si>
-  <si>
     <t>Prerequisites</t>
   </si>
   <si>
@@ -764,27 +755,12 @@
     <t>MT1002</t>
   </si>
   <si>
-    <t>MT1002 or co-requisite MT1010.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MT1002</t>
-  </si>
-  <si>
-    <t>MT2503.</t>
-  </si>
-  <si>
-    <t>MT2504.</t>
-  </si>
-  <si>
     <t>MT3501 or MT3502 or MT3503 or MT3504 or MT3505 or MT3506 or MT3507 or MT3508</t>
   </si>
   <si>
     <t>co-requisite MT3510</t>
   </si>
   <si>
-    <t>MT 3504 and (MT2506 or PH3081)</t>
-  </si>
-  <si>
     <t>MT2506 and MT3504</t>
   </si>
   <si>
@@ -833,9 +809,6 @@
     <t>MT5865 or MT5825</t>
   </si>
   <si>
-    <t>EC2203.</t>
-  </si>
-  <si>
     <t>Not on a Computer Science programme</t>
   </si>
   <si>
@@ -854,9 +827,6 @@
     <t>co-requisite MT4113 and (MT3507 or MT3508)</t>
   </si>
   <si>
-    <t xml:space="preserve"> MT5802</t>
-  </si>
-  <si>
     <t>MT5806</t>
   </si>
   <si>
@@ -948,6 +918,24 @@
   </si>
   <si>
     <t>6pm - 9pm Wed</t>
+  </si>
+  <si>
+    <t>Module code</t>
+  </si>
+  <si>
+    <t>Module name</t>
+  </si>
+  <si>
+    <t>Alternate years</t>
+  </si>
+  <si>
+    <t>MT3504 and (MT2506 or PH3081)</t>
+  </si>
+  <si>
+    <t>EC2203</t>
+  </si>
+  <si>
+    <t>MT5802</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1322,7 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1352,2477 +1340,2477 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>265</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>248</v>
+        <v>297</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="F74" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="H93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can now check for timetable clashes
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC1F0AE-7C71-C147-BEAD-70C6BD12C2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC786C20-6335-6542-9B56-82DC6F566B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BA51B351-0636-AB4E-9862-84BEC7942AF0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="292">
   <si>
     <t>Year</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Techniques of Applied Mathematics</t>
   </si>
   <si>
-    <t>MT2506, MT3504</t>
-  </si>
-  <si>
     <t>PH3081</t>
   </si>
   <si>
@@ -623,9 +620,6 @@
     <t>Semigroups</t>
   </si>
   <si>
-    <t>To be confirmed</t>
-  </si>
-  <si>
     <t>MT5864</t>
   </si>
   <si>
@@ -704,15 +698,6 @@
     <t>S2</t>
   </si>
   <si>
-    <t>Mon (even weeks), Tue and Thu</t>
-  </si>
-  <si>
-    <t>3:30pm-5pm Mon, Thur, Fri</t>
-  </si>
-  <si>
-    <t>11am Mons (odd weeks), Wed and 4pm Fri</t>
-  </si>
-  <si>
     <t>12noon Mon (odd weeks), Wed, Fri</t>
   </si>
   <si>
@@ -866,60 +851,18 @@
     <t>CS5014</t>
   </si>
   <si>
-    <t>9am Mon (even weeks), Tue and Thu</t>
-  </si>
-  <si>
-    <t>11am Mon (even weeks), Tue and Thu</t>
-  </si>
-  <si>
-    <t>9am Mon (odd weeks), Wed and Fri</t>
-  </si>
-  <si>
-    <t>11am Mon (odd weeks), Wed and Fri</t>
-  </si>
-  <si>
-    <t>10am Mon (odd weeks), Wed and Fri</t>
-  </si>
-  <si>
-    <t>10am Wed and Fri (odd weeks)</t>
-  </si>
-  <si>
-    <t>10am Mon (even weeks), Tue and Thu</t>
-  </si>
-  <si>
-    <t>12noon Mon (odd weeks), Wed and Fri</t>
-  </si>
-  <si>
-    <t>12noon Mon (even weeks), Tue and Thu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12noon Mon (even weeks), Tue and Thur</t>
-  </si>
-  <si>
     <t>12noon Mon, Tue, Thur</t>
   </si>
   <si>
     <t>12noon Mon (even weeks), Tue, Thu</t>
   </si>
   <si>
-    <t>12noon Mon (odd weeks), Wed, Fri.</t>
-  </si>
-  <si>
     <t>12noon Mons (even weeks), Tue, Thu</t>
   </si>
   <si>
     <t>12noon Mons (odd weeks), Wed, Fri</t>
   </si>
   <si>
-    <t>12noon Mon (odd weeks) and Wed, 12noon - 2pm Fri</t>
-  </si>
-  <si>
-    <t>12noon Mon (odd weeks), Wed, Fri, and 2pm Fri</t>
-  </si>
-  <si>
-    <t>6pm - 9pm Wed</t>
-  </si>
-  <si>
     <t>Module code</t>
   </si>
   <si>
@@ -936,6 +879,39 @@
   </si>
   <si>
     <t>MT5802</t>
+  </si>
+  <si>
+    <t>12noon Mon (odd weeks), Wed, Fri, 1pm Fri</t>
+  </si>
+  <si>
+    <t>12noon Mon (odd weeks), Wed, Fri, 2pm Fri</t>
+  </si>
+  <si>
+    <t>6pm Wed, 7pm Wed, 9pm Wed</t>
+  </si>
+  <si>
+    <t>3pm Mon, 3pm Thur, 3pm Fri, 4pm Mon, 4pm Thur, 4pm Fri</t>
+  </si>
+  <si>
+    <t>11am Mon (even weeks), Tue, Thu</t>
+  </si>
+  <si>
+    <t>9am Mon (odd weeks), Wed, Fri</t>
+  </si>
+  <si>
+    <t>11am Mons (odd weeks), Wed, 4pm Fri</t>
+  </si>
+  <si>
+    <t>9am Mon (even weeks), Tue, Thu</t>
+  </si>
+  <si>
+    <t>10am Wed, Fri (odd weeks)</t>
+  </si>
+  <si>
+    <t>12noon Mon (even weeks), Tue, Thur</t>
+  </si>
+  <si>
+    <t>10am Mon (even weeks), Tue, Thur</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H85" sqref="H85"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1340,10 +1316,10 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1355,7 +1331,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -1375,16 +1351,16 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1399,16 +1375,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1423,16 +1399,16 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1447,16 +1423,16 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1471,16 +1447,16 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1494,16 +1470,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>224</v>
+        <v>287</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1518,16 +1494,16 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>279</v>
+        <v>177</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1542,10 +1518,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -1566,10 +1542,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
@@ -1590,10 +1566,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -1602,7 +1578,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1616,10 +1592,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -1637,10 +1613,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -1661,10 +1637,10 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -1685,10 +1661,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>
@@ -1709,10 +1685,10 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -1732,10 +1708,10 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>279</v>
+        <v>177</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>8</v>
@@ -1756,36 +1732,36 @@
         <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>279</v>
+        <v>177</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
@@ -1797,19 +1773,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -1820,41 +1796,41 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>280</v>
+        <v>223</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
@@ -1865,19 +1841,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
@@ -1889,19 +1865,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
@@ -1913,69 +1889,69 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>8</v>
@@ -1986,144 +1962,144 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>279</v>
+        <v>177</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>32</v>
@@ -2132,168 +2108,168 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>280</v>
+        <v>223</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>27</v>
@@ -2301,142 +2277,142 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>280</v>
+        <v>223</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>27</v>
@@ -2445,22 +2421,22 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>21</v>
@@ -2469,22 +2445,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>13</v>
@@ -2493,22 +2469,22 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>21</v>
@@ -2517,116 +2493,116 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>8</v>
@@ -2638,64 +2614,64 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="C56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="C57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
@@ -2704,48 +2680,48 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>280</v>
+        <v>223</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>21</v>
@@ -2754,83 +2730,83 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="C60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="C63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
@@ -2841,16 +2817,16 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
@@ -2861,16 +2837,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
@@ -2878,21 +2854,21 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="C66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
@@ -2903,60 +2879,60 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="C67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="C69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
@@ -2967,271 +2943,271 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H70" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="H74" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="C76" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="C77" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="C78" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="C80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>8</v>
@@ -3240,102 +3216,102 @@
         <v>29</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="C81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="F82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="C84" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>8</v>
@@ -3344,24 +3320,24 @@
         <v>32</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>8</v>
@@ -3373,169 +3349,167 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>288</v>
+        <v>220</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="C89" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>195</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>8</v>
@@ -3544,149 +3518,149 @@
         <v>27</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
@@ -3697,43 +3671,43 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>8</v>
@@ -3743,74 +3717,74 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parsing folders and fixing errors
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC786C20-6335-6542-9B56-82DC6F566B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369803A3-17F3-3A45-A838-12D7BF37B37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BA51B351-0636-AB4E-9862-84BEC7942AF0}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="38400" windowHeight="21100" xr2:uid="{BA51B351-0636-AB4E-9862-84BEC7942AF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="290">
   <si>
     <t>Year</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Dynamical Systems</t>
   </si>
   <si>
-    <t>Pass MT3504</t>
-  </si>
-  <si>
     <t>MT4509</t>
   </si>
   <si>
@@ -710,18 +707,12 @@
     <t>10am Mon (odd weeks), Wed, Fri</t>
   </si>
   <si>
-    <t>Lectures - Mon (odd weeks), Wed, Fri</t>
-  </si>
-  <si>
     <t>10am, Mon (odd weeks), Wed, Fri</t>
   </si>
   <si>
     <t>9am Mon (even), Tue, Thu</t>
   </si>
   <si>
-    <t>3pm Mon, Tue, Thur, Fri</t>
-  </si>
-  <si>
     <t>10:00am Mon, Wed, Fri</t>
   </si>
   <si>
@@ -905,13 +896,16 @@
     <t>9am Mon (even weeks), Tue, Thu</t>
   </si>
   <si>
-    <t>10am Wed, Fri (odd weeks)</t>
-  </si>
-  <si>
     <t>12noon Mon (even weeks), Tue, Thur</t>
   </si>
   <si>
     <t>10am Mon (even weeks), Tue, Thur</t>
+  </si>
+  <si>
+    <t>10am Wed (odd weeks), 10am Fri (odd weeks)</t>
+  </si>
+  <si>
+    <t>3pm Mon, 3pm Tue, 3pm Thur, 3pm Fri</t>
   </si>
 </sst>
 </file>
@@ -1297,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1309,17 +1303,17 @@
     <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="59.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="52.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="69.1640625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1331,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -1351,16 +1345,16 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1375,16 +1369,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1399,16 +1393,16 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1423,16 +1417,16 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1447,16 +1441,16 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1470,16 +1464,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1494,16 +1488,16 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1518,10 +1512,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -1542,10 +1536,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
@@ -1566,10 +1560,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -1578,7 +1572,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,10 +1586,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -1613,10 +1607,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -1637,10 +1631,10 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -1661,10 +1655,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>
@@ -1685,10 +1679,10 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -1708,10 +1702,10 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>8</v>
@@ -1732,16 +1726,16 @@
         <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>38</v>
@@ -1758,10 +1752,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
@@ -1782,10 +1776,10 @@
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -1805,14 +1799,14 @@
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1827,10 +1821,10 @@
         <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
@@ -1850,10 +1844,10 @@
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
@@ -1874,10 +1868,10 @@
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
@@ -1898,10 +1892,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>8</v>
@@ -1922,19 +1916,19 @@
         <v>56</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1948,10 +1942,10 @@
         <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>8</v>
@@ -1971,10 +1965,10 @@
         <v>56</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>61</v>
@@ -1995,16 +1989,16 @@
         <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>65</v>
@@ -2021,82 +2015,82 @@
         <v>56</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="C32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>61</v>
@@ -2108,165 +2102,165 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>61</v>
@@ -2277,139 +2271,139 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>61</v>
@@ -2421,19 +2415,19 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>61</v>
@@ -2445,19 +2439,19 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>61</v>
@@ -2469,19 +2463,19 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>61</v>
@@ -2493,116 +2487,116 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>8</v>
@@ -2614,64 +2608,64 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="C56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
@@ -2680,19 +2674,19 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>61</v>
@@ -2701,24 +2695,24 @@
         <v>39</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>61</v>
@@ -2730,83 +2724,83 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="C60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="C63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
@@ -2817,16 +2811,16 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
@@ -2837,16 +2831,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
@@ -2854,21 +2848,21 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
@@ -2879,60 +2873,60 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="C67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="C69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
@@ -2943,271 +2937,271 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H70" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>227</v>
+        <v>289</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="H74" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C76" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="C80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>8</v>
@@ -3216,102 +3210,102 @@
         <v>29</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="C81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="C84" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>8</v>
@@ -3320,24 +3314,24 @@
         <v>32</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>8</v>
@@ -3349,141 +3343,141 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="C91" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>8</v>
@@ -3492,24 +3486,24 @@
         <v>47</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C92" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>8</v>
@@ -3518,100 +3512,100 @@
         <v>27</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="C93" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="C94" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="C95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="C96" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>61</v>
@@ -3620,47 +3614,47 @@
         <v>34</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C98" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
@@ -3671,43 +3665,43 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="C99" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="C100" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>8</v>
@@ -3717,74 +3711,74 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="C101" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="C102" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="C103" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduced error handling for fileformatting issues and improved output
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369803A3-17F3-3A45-A838-12D7BF37B37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F810AA8-294F-3A45-A109-489372A6B9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="38400" windowHeight="21100" xr2:uid="{BA51B351-0636-AB4E-9862-84BEC7942AF0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BA51B351-0636-AB4E-9862-84BEC7942AF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -710,12 +710,6 @@
     <t>10am, Mon (odd weeks), Wed, Fri</t>
   </si>
   <si>
-    <t>9am Mon (even), Tue, Thu</t>
-  </si>
-  <si>
-    <t>10:00am Mon, Wed, Fri</t>
-  </si>
-  <si>
     <t>2pm Thur</t>
   </si>
   <si>
@@ -906,6 +900,12 @@
   </si>
   <si>
     <t>3pm Mon, 3pm Tue, 3pm Thur, 3pm Fri</t>
+  </si>
+  <si>
+    <t>2024/2025</t>
+  </si>
+  <si>
+    <t>10am Mon, Wed, Fri</t>
   </si>
 </sst>
 </file>
@@ -1291,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1310,10 +1310,10 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -1354,7 +1354,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1372,13 +1372,13 @@
         <v>218</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1396,13 +1396,13 @@
         <v>217</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1420,13 +1420,13 @@
         <v>217</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1444,13 +1444,13 @@
         <v>218</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1467,13 +1467,13 @@
         <v>217</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1497,7 +1497,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1515,7 +1515,7 @@
         <v>218</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -1563,7 +1563,7 @@
         <v>218</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -1572,7 +1572,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>217</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -1610,7 +1610,7 @@
         <v>217</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -1634,7 +1634,7 @@
         <v>217</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -1682,7 +1682,7 @@
         <v>217</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -1735,7 +1735,7 @@
         <v>8</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>38</v>
@@ -1779,7 +1779,7 @@
         <v>218</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -1806,7 +1806,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1847,7 +1847,7 @@
         <v>218</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
@@ -1871,7 +1871,7 @@
         <v>218</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
@@ -1895,7 +1895,7 @@
         <v>217</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>8</v>
@@ -1919,16 +1919,16 @@
         <v>217</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
         <v>217</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>8</v>
@@ -1998,7 +1998,7 @@
         <v>61</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>65</v>
@@ -2042,13 +2042,13 @@
         <v>218</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -2072,7 +2072,7 @@
         <v>8</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2090,7 +2090,7 @@
         <v>217</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>61</v>
@@ -2120,7 +2120,7 @@
         <v>61</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>76</v>
@@ -2140,7 +2140,7 @@
         <v>218</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>61</v>
@@ -2188,7 +2188,7 @@
         <v>218</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>61</v>
@@ -2283,7 +2283,7 @@
         <v>218</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>61</v>
@@ -2331,7 +2331,7 @@
         <v>218</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>61</v>
@@ -2451,7 +2451,7 @@
         <v>217</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>61</v>
@@ -2475,7 +2475,7 @@
         <v>217</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>61</v>
@@ -2508,7 +2508,7 @@
         <v>102</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2548,7 +2548,7 @@
         <v>218</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>8</v>
@@ -2596,7 +2596,7 @@
         <v>218</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>8</v>
@@ -2736,13 +2736,13 @@
         <v>218</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H60" s="1"/>
     </row>
@@ -2949,7 +2949,7 @@
         <v>217</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>8</v>
@@ -2999,7 +2999,7 @@
         <v>218</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>8</v>
@@ -3025,16 +3025,16 @@
         <v>217</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
         <v>217</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>8</v>
@@ -3060,7 +3060,7 @@
         <v>159</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3077,16 +3077,16 @@
         <v>217</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3103,16 +3103,16 @@
         <v>218</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>218</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>225</v>
+        <v>289</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>61</v>
@@ -3147,19 +3147,19 @@
         <v>167</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>56</v>
+        <v>288</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H78" s="1"/>
     </row>
@@ -3210,7 +3210,7 @@
         <v>29</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3227,16 +3227,16 @@
         <v>218</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3262,7 +3262,7 @@
         <v>68</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
         <v>217</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>8</v>
@@ -3288,7 +3288,7 @@
         <v>70</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3314,7 +3314,7 @@
         <v>32</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3361,7 +3361,7 @@
         <v>8</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H86" s="1"/>
     </row>
@@ -3385,7 +3385,7 @@
         <v>8</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H87" s="1"/>
     </row>
@@ -3409,10 +3409,10 @@
         <v>61</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>61</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H89" s="1"/>
     </row>
@@ -3457,10 +3457,10 @@
         <v>61</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
         <v>47</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3512,7 +3512,7 @@
         <v>27</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3529,13 +3529,13 @@
         <v>217</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H93" s="1"/>
     </row>
@@ -3553,16 +3553,16 @@
         <v>218</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3585,10 +3585,10 @@
         <v>61</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3614,7 +3614,7 @@
         <v>34</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3631,16 +3631,16 @@
         <v>218</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>224</v>
+        <v>283</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3684,7 +3684,7 @@
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3701,7 +3701,7 @@
         <v>217</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>8</v>
@@ -3723,7 +3723,7 @@
         <v>217</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>8</v>
@@ -3747,7 +3747,7 @@
         <v>217</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>8</v>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated catalogue with new modules (MT4554,MT5868,MT5869) and corrected minor timetable/pre-req errors
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwrj1/Downloads/Code-temp/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F810AA8-294F-3A45-A109-489372A6B9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132D6B77-D424-9243-A605-A4509E6C0089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BA51B351-0636-AB4E-9862-84BEC7942AF0}"/>
+    <workbookView xWindow="0" yWindow="13080" windowWidth="51200" windowHeight="13600" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="296">
   <si>
     <t>Year</t>
   </si>
@@ -173,12 +173,6 @@
     <t>Introduction to Mathematical Computing</t>
   </si>
   <si>
-    <t>MT3802</t>
-  </si>
-  <si>
-    <t>Numerical Analysis</t>
-  </si>
-  <si>
     <t>MT4003</t>
   </si>
   <si>
@@ -710,9 +704,6 @@
     <t>10am, Mon (odd weeks), Wed, Fri</t>
   </si>
   <si>
-    <t>2pm Thur</t>
-  </si>
-  <si>
     <t>1pm Mon, Tue, Thu</t>
   </si>
   <si>
@@ -728,9 +719,6 @@
     <t>MT3501 or MT3502 or MT3503 or MT3504 or MT3505 or MT3506 or MT3507 or MT3508</t>
   </si>
   <si>
-    <t>co-requisite MT3510</t>
-  </si>
-  <si>
     <t>MT2506 and MT3504</t>
   </si>
   <si>
@@ -836,9 +824,6 @@
     <t>CS5014</t>
   </si>
   <si>
-    <t>12noon Mon, Tue, Thur</t>
-  </si>
-  <si>
     <t>12noon Mon (even weeks), Tue, Thu</t>
   </si>
   <si>
@@ -875,9 +860,6 @@
     <t>6pm Wed, 7pm Wed, 9pm Wed</t>
   </si>
   <si>
-    <t>3pm Mon, 3pm Thur, 3pm Fri, 4pm Mon, 4pm Thur, 4pm Fri</t>
-  </si>
-  <si>
     <t>11am Mon (even weeks), Tue, Thu</t>
   </si>
   <si>
@@ -890,22 +872,58 @@
     <t>9am Mon (even weeks), Tue, Thu</t>
   </si>
   <si>
-    <t>12noon Mon (even weeks), Tue, Thur</t>
-  </si>
-  <si>
-    <t>10am Mon (even weeks), Tue, Thur</t>
-  </si>
-  <si>
-    <t>10am Wed (odd weeks), 10am Fri (odd weeks)</t>
-  </si>
-  <si>
-    <t>3pm Mon, 3pm Tue, 3pm Thur, 3pm Fri</t>
-  </si>
-  <si>
     <t>2024/2025</t>
   </si>
   <si>
     <t>10am Mon, Wed, Fri</t>
+  </si>
+  <si>
+    <t>MT4554</t>
+  </si>
+  <si>
+    <t>Game Theory</t>
+  </si>
+  <si>
+    <t>(MT2503 and MT2504) or EC3304</t>
+  </si>
+  <si>
+    <t>MT5868</t>
+  </si>
+  <si>
+    <t>Advanced Ring Theory</t>
+  </si>
+  <si>
+    <t>MT5869</t>
+  </si>
+  <si>
+    <t>Geometric Group Theory</t>
+  </si>
+  <si>
+    <t>MT4003 and MT4526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10am Wed, 10am Fri </t>
+  </si>
+  <si>
+    <t>3pm Mon, 3pm Tue, 3pm Thu, 3pm Fri</t>
+  </si>
+  <si>
+    <t>12noon Mon, Tue, Thu</t>
+  </si>
+  <si>
+    <t>2pm Thu</t>
+  </si>
+  <si>
+    <t>3pm Mon, 3pm Thu, 3pm Fri, 4pm Mon, 4pm Thu, 4pm Fri</t>
+  </si>
+  <si>
+    <t>MT3510 and co-requisite MT3504</t>
+  </si>
+  <si>
+    <t>MT2508 and MT3510</t>
+  </si>
+  <si>
+    <t>2025/2026</t>
   </si>
 </sst>
 </file>
@@ -1289,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1310,10 +1328,10 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1325,7 +1343,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -1345,16 +1363,16 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1369,16 +1387,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1393,16 +1411,16 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1417,16 +1435,16 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1441,16 +1459,16 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1464,16 +1482,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1488,16 +1506,16 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1512,10 +1530,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -1536,10 +1554,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
@@ -1560,10 +1578,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -1572,7 +1590,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1586,10 +1604,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -1607,10 +1625,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -1631,10 +1649,10 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -1655,10 +1673,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>
@@ -1679,10 +1697,10 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -1702,10 +1720,10 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>8</v>
@@ -1726,16 +1744,16 @@
         <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>38</v>
@@ -1752,10 +1770,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
@@ -1776,10 +1794,10 @@
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -1799,14 +1817,14 @@
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1821,17 +1839,18 @@
         <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>222</v>
+        <v>277</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1844,16 +1863,16 @@
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -1868,67 +1887,66 @@
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="1"/>
+        <v>293</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>247</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1939,70 +1957,71 @@
         <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>21</v>
+        <v>59</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>219</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="H28" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -2012,19 +2031,19 @@
         <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>221</v>
+        <v>274</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -2039,16 +2058,16 @@
         <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>280</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -2063,16 +2082,16 @@
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>176</v>
+        <v>277</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>231</v>
+        <v>32</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2087,44 +2106,44 @@
         <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>283</v>
+        <v>219</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H33" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -2134,43 +2153,43 @@
         <v>78</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="H36" s="1"/>
     </row>
@@ -2182,43 +2201,43 @@
         <v>83</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -2230,577 +2249,560 @@
         <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>7</v>
+        <v>295</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H43" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>56</v>
+        <v>278</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H44" s="1"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>278</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>98</v>
+        <v>280</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>99</v>
+        <v>281</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>21</v>
+        <v>282</v>
       </c>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>221</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>248</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>221</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>277</v>
+        <v>220</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H52" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>32</v>
+        <v>229</v>
       </c>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H56" s="1"/>
+        <v>129</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>123</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>281</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>130</v>
+        <v>216</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>131</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
@@ -2811,394 +2813,422 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E64" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="F64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
+      <c r="G64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="F65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="G65" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E66" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="F66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
+      <c r="G66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E67" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="F67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H67" s="1"/>
+        <v>230</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E68" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="F68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H68" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E69" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="F69" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
+      <c r="G69" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>102</v>
+        <v>232</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>148</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>219</v>
+        <v>279</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>7</v>
+        <v>278</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>154</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>287</v>
+        <v>220</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>249</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="F74" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>266</v>
+        <v>174</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>236</v>
+        <v>66</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H77" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>288</v>
+        <v>7</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="G78" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>219</v>
@@ -3207,182 +3237,178 @@
         <v>8</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>275</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="H80" s="1"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>267</v>
+        <v>220</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>253</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="H81" s="1"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="F82" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>68</v>
+        <v>236</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="F83" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>255</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>220</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>32</v>
+        <v>238</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H85" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="H86" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>222</v>
+        <v>263</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>239</v>
@@ -3391,22 +3417,22 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>240</v>
@@ -3417,368 +3443,266 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>189</v>
+        <v>283</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>190</v>
+        <v>284</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>219</v>
+        <v>274</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>241</v>
+        <v>34</v>
       </c>
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>191</v>
+        <v>285</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>192</v>
+        <v>286</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>56</v>
+        <v>278</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E90" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="F90" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>258</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>47</v>
+        <v>241</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="H93" s="1"/>
+        <v>242</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>269</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>261</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>223</v>
+        <v>174</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>245</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G95" s="1"/>
       <c r="H95" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>176</v>
+        <v>222</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>263</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>283</v>
+        <v>223</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>246</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G97" s="1"/>
       <c r="H97" s="1" t="s">
-        <v>264</v>
+        <v>213</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E98" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="F98" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
+      <c r="H98" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding recent timetable changes
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwrj1/Downloads/Code-temp/StA_Advising/module_catalogue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF12DEF-F0D9-A64C-B032-FB1AF595F91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7BE6B9-5635-0647-94D5-EFE23935520C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="13080" windowWidth="51200" windowHeight="13600" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="297">
   <si>
     <t>Year</t>
   </si>
@@ -924,6 +924,9 @@
   </si>
   <si>
     <t>2025/2026</t>
+  </si>
+  <si>
+    <t>11am Mon (odd weeks), Tue, Thu</t>
   </si>
 </sst>
 </file>
@@ -1309,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="B75" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3555,7 +3558,7 @@
         <v>216</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
correcting timetable change in .xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7BE6B9-5635-0647-94D5-EFE23935520C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D63E8FE-A27D-8A4A-8719-DBBF9D3B70AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="296">
   <si>
     <t>Year</t>
   </si>
@@ -924,9 +924,6 @@
   </si>
   <si>
     <t>2025/2026</t>
-  </si>
-  <si>
-    <t>11am Mon (odd weeks), Tue, Thu</t>
   </si>
 </sst>
 </file>
@@ -3558,7 +3555,7 @@
         <v>216</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>296</v>
+        <v>174</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
fixing entry for MT5756 Medical Statistics
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D63E8FE-A27D-8A4A-8719-DBBF9D3B70AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CDD80B-400F-8144-9366-AD46A4E61AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
@@ -1309,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B75" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="B59" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3008,7 +3008,7 @@
         <v>279</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
fixing MT5856 prerequisites (MT3802 is no longer required)
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CDD80B-400F-8144-9366-AD46A4E61AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6BC743-15A7-EA4C-86AF-11AAD9C0F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="295">
   <si>
     <t>Year</t>
   </si>
@@ -741,9 +741,6 @@
   </si>
   <si>
     <t>MT2508 and MT3504</t>
-  </si>
-  <si>
-    <t>MT3504 and MT3802</t>
   </si>
   <si>
     <t>MT4514 or MT4516</t>
@@ -1309,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B59" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="C64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1325,10 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1343,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -1390,7 +1387,7 @@
         <v>216</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -1414,7 +1411,7 @@
         <v>215</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
@@ -1438,7 +1435,7 @@
         <v>215</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
@@ -1462,7 +1459,7 @@
         <v>216</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
@@ -1485,7 +1482,7 @@
         <v>215</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -1533,7 +1530,7 @@
         <v>216</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -1581,7 +1578,7 @@
         <v>216</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -1590,7 +1587,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1607,7 +1604,7 @@
         <v>215</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -1628,7 +1625,7 @@
         <v>215</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -1652,7 +1649,7 @@
         <v>215</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -1700,7 +1697,7 @@
         <v>215</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -1797,7 +1794,7 @@
         <v>216</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -1842,7 +1839,7 @@
         <v>216</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
@@ -1866,7 +1863,7 @@
         <v>216</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
@@ -1890,7 +1887,7 @@
         <v>215</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
@@ -1914,16 +1911,16 @@
         <v>215</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1940,13 +1937,13 @@
         <v>215</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1993,7 +1990,7 @@
         <v>59</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>63</v>
@@ -2037,7 +2034,7 @@
         <v>216</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>8</v>
@@ -2085,7 +2082,7 @@
         <v>215</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>59</v>
@@ -2135,7 +2132,7 @@
         <v>216</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>59</v>
@@ -2183,7 +2180,7 @@
         <v>216</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>59</v>
@@ -2303,7 +2300,7 @@
         <v>215</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>59</v>
@@ -2321,13 +2318,13 @@
         <v>97</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>215</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>59</v>
@@ -2360,7 +2357,7 @@
         <v>100</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2371,7 +2368,7 @@
         <v>102</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>216</v>
@@ -2394,13 +2391,13 @@
         <v>104</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>216</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>8</v>
@@ -2448,7 +2445,7 @@
         <v>216</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>8</v>
@@ -2486,10 +2483,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>54</v>
@@ -2498,13 +2495,13 @@
         <v>215</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H49" s="1"/>
     </row>
@@ -2612,7 +2609,7 @@
         <v>216</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>8</v>
@@ -2875,7 +2872,7 @@
         <v>216</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>8</v>
@@ -2901,7 +2898,7 @@
         <v>215</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>8</v>
@@ -2910,7 +2907,7 @@
         <v>230</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2927,7 +2924,7 @@
         <v>215</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>8</v>
@@ -2936,7 +2933,7 @@
         <v>157</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2953,7 +2950,7 @@
         <v>215</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>8</v>
@@ -2962,7 +2959,7 @@
         <v>231</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2979,7 +2976,7 @@
         <v>216</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>8</v>
@@ -2988,7 +2985,7 @@
         <v>232</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3005,7 +3002,7 @@
         <v>216</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>8</v>
@@ -3023,19 +3020,19 @@
         <v>165</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H72" s="1"/>
     </row>
@@ -3086,7 +3083,7 @@
         <v>29</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3103,7 +3100,7 @@
         <v>216</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>8</v>
@@ -3112,7 +3109,7 @@
         <v>233</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3138,7 +3135,7 @@
         <v>66</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3155,7 +3152,7 @@
         <v>215</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>8</v>
@@ -3164,7 +3161,7 @@
         <v>68</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3190,7 +3187,7 @@
         <v>32</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3261,7 +3258,7 @@
         <v>8</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>235</v>
+        <v>32</v>
       </c>
       <c r="H81" s="1"/>
     </row>
@@ -3285,10 +3282,10 @@
         <v>59</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3311,7 +3308,7 @@
         <v>59</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H83" s="1"/>
     </row>
@@ -3333,10 +3330,10 @@
         <v>59</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3362,7 +3359,7 @@
         <v>45</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3388,7 +3385,7 @@
         <v>27</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3405,13 +3402,13 @@
         <v>215</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H87" s="1"/>
     </row>
@@ -3429,24 +3426,24 @@
         <v>216</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>284</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>54</v>
@@ -3455,7 +3452,7 @@
         <v>215</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>59</v>
@@ -3467,13 +3464,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>215</v>
@@ -3485,7 +3482,7 @@
         <v>59</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H90" s="1"/>
     </row>
@@ -3509,10 +3506,10 @@
         <v>59</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3538,7 +3535,7 @@
         <v>34</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3561,10 +3558,10 @@
         <v>59</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3608,7 +3605,7 @@
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3702,7 +3699,7 @@
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to prereqs/antireqs approved -	MT5846 prereqs/antireqs -	MT5766 prereq -	MT5763 prereqs/antireqs -	MT4551 prereq -	MT4005 prereq
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/Advising-tool/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{8C6BC743-15A7-EA4C-86AF-11AAD9C0F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE4132F7-8BD1-4D43-9C80-6B69E03A5E9F}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{8C6BC743-15A7-EA4C-86AF-11AAD9C0F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C549DC9-EEB9-1D44-B859-0F4171AA302E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="49640" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="291">
   <si>
     <t>Module code</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Linear and Nonlinear Waves</t>
   </si>
   <si>
-    <t>(MT2506 or PH3081) and (MT3503 or MT3504)</t>
-  </si>
-  <si>
     <t>MT4112</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>Financial Mathematics</t>
   </si>
   <si>
-    <t>MT2503 and (MT1007 or MT2504 or EC2203) and MT3504</t>
-  </si>
-  <si>
     <t>MT4552</t>
   </si>
   <si>
@@ -632,9 +626,6 @@
     <t>Software for Data Analysis</t>
   </si>
   <si>
-    <t>MT1007 or MT3507 or MT3508 or co-requisite MT5762</t>
-  </si>
-  <si>
     <t>MT5764</t>
   </si>
   <si>
@@ -662,9 +653,6 @@
     <t>2pm Thu</t>
   </si>
   <si>
-    <t>co-requisite MT4113 and (MT3507 or MT3508)</t>
-  </si>
-  <si>
     <t>MT5767</t>
   </si>
   <si>
@@ -686,12 +674,6 @@
     <t>Advanced Computational Techniques</t>
   </si>
   <si>
-    <t>MT3802 and MT4112</t>
-  </si>
-  <si>
-    <t>MT5806</t>
-  </si>
-  <si>
     <t>MT5849</t>
   </si>
   <si>
@@ -918,6 +900,15 @@
   </si>
   <si>
     <t>MT1007 or MT2508 or EC2203 or PH3012</t>
+  </si>
+  <si>
+    <t>(MT2506 or PH3081) and MT3504</t>
+  </si>
+  <si>
+    <t>MT3504 and (MT2504 or EC2203 or PH3012)</t>
+  </si>
+  <si>
+    <t>co-requisite MT4113 or MT5763</t>
   </si>
 </sst>
 </file>
@@ -1307,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:XFD96"/>
+    <sheetView tabSelected="1" topLeftCell="D60" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1891,71 +1882,71 @@
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>68</v>
+        <v>288</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -1964,57 +1955,57 @@
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>47</v>
@@ -2023,10 +2014,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>10</v>
@@ -2047,10 +2038,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>10</v>
@@ -2071,10 +2062,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>10</v>
@@ -2086,7 +2077,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>47</v>
@@ -2095,39 +2086,39 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>15</v>
@@ -2136,43 +2127,43 @@
         <v>21</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>10</v>
@@ -2184,79 +2175,79 @@
         <v>21</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="C39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>42</v>
@@ -2265,11 +2256,11 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="C40" s="1" t="s">
         <v>10</v>
       </c>
@@ -2277,10 +2268,10 @@
         <v>15</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>34</v>
@@ -2289,13 +2280,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -2304,7 +2295,7 @@
         <v>16</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>23</v>
@@ -2313,13 +2304,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -2328,7 +2319,7 @@
         <v>31</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>34</v>
@@ -2337,107 +2328,107 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="D44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="C46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>137</v>
+        <v>289</v>
       </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>10</v>
@@ -2458,39 +2449,39 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -2499,47 +2490,47 @@
         <v>31</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
@@ -2548,36 +2539,36 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>10</v>
@@ -2589,7 +2580,7 @@
         <v>16</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>34</v>
@@ -2598,10 +2589,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>10</v>
@@ -2616,65 +2607,65 @@
         <v>13</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
@@ -2685,16 +2676,16 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
@@ -2705,16 +2696,16 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
@@ -2722,21 +2713,21 @@
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
@@ -2747,10 +2738,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>10</v>
@@ -2763,16 +2754,16 @@
         <v>13</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>10</v>
@@ -2785,22 +2776,22 @@
         <v>13</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
@@ -2811,36 +2802,36 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>10</v>
@@ -2855,16 +2846,16 @@
         <v>13</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>10</v>
@@ -2879,70 +2870,70 @@
         <v>13</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="F67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" s="1" t="s">
+      <c r="H67" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="F68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="1" t="s">
+      <c r="H68" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>10</v>
@@ -2957,18 +2948,18 @@
         <v>13</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>195</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>10</v>
@@ -2983,66 +2974,66 @@
         <v>13</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>208</v>
+        <v>290</v>
       </c>
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>10</v>
@@ -3051,22 +3042,22 @@
         <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>10</v>
@@ -3084,15 +3075,15 @@
         <v>44</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>10</v>
@@ -3107,18 +3098,16 @@
         <v>13</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>217</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H75" s="1"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>10</v>
@@ -3133,18 +3122,18 @@
         <v>13</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>10</v>
@@ -3159,18 +3148,18 @@
         <v>13</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>10</v>
@@ -3188,15 +3177,15 @@
         <v>47</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>10</v>
@@ -3217,10 +3206,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>10</v>
@@ -3229,22 +3218,22 @@
         <v>11</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H80" s="1"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>10</v>
@@ -3265,13 +3254,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>15</v>
@@ -3280,24 +3269,24 @@
         <v>12</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
@@ -3306,45 +3295,45 @@
         <v>12</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>10</v>
@@ -3353,24 +3342,24 @@
         <v>11</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>62</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>10</v>
@@ -3388,15 +3377,15 @@
         <v>42</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>10</v>
@@ -3408,19 +3397,19 @@
         <v>21</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>10</v>
@@ -3432,24 +3421,24 @@
         <v>12</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>11</v>
@@ -3458,7 +3447,7 @@
         <v>16</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>49</v>
@@ -3467,34 +3456,34 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>10</v>
@@ -3503,24 +3492,24 @@
         <v>15</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>10</v>
@@ -3532,24 +3521,24 @@
         <v>28</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>15</v>
@@ -3558,27 +3547,27 @@
         <v>28</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
@@ -3589,10 +3578,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>10</v>
@@ -3608,15 +3597,15 @@
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>10</v>
@@ -3625,22 +3614,22 @@
         <v>11</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>10</v>
@@ -3649,48 +3638,48 @@
         <v>11</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>15</v>
@@ -3699,21 +3688,21 @@
         <v>22</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>11</v>
@@ -3722,10 +3711,10 @@
         <v>31</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated catalogue - changed year for modules that will newly start to alternate (MT4005, MT4531, MT5731) - updated pre-reqs/co-reqs for MT4501 and MT4561
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/Advising-tool/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{8C6BC743-15A7-EA4C-86AF-11AAD9C0F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C549DC9-EEB9-1D44-B859-0F4171AA302E}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{8C6BC743-15A7-EA4C-86AF-11AAD9C0F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85D4F195-4770-B74A-84BB-2DA5C2EC65E8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="49640" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="291">
   <si>
     <t>Module code</t>
   </si>
@@ -899,9 +899,6 @@
     <t>The History and Future of Data</t>
   </si>
   <si>
-    <t>MT1007 or MT2508 or EC2203 or PH3012</t>
-  </si>
-  <si>
     <t>(MT2506 or PH3081) and MT3504</t>
   </si>
   <si>
@@ -909,6 +906,9 @@
   </si>
   <si>
     <t>co-requisite MT4113 or MT5763</t>
+  </si>
+  <si>
+    <t>MT1007 or MT2508 or EC2203 or PH3012 and (MT3501 or MT3502 or MT3503 or MT3504 or MT3505 or MT3506 or MT3507 or MT3508)</t>
   </si>
 </sst>
 </file>
@@ -995,14 +995,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1040,7 +1036,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1146,7 +1142,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1288,7 +1284,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1298,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D60" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1306,7 @@
     <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="59.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" customWidth="1"/>
-    <col min="7" max="7" width="52.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="138" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="69.1640625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -1873,7 +1869,7 @@
         <v>67</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>15</v>
@@ -1885,7 +1881,7 @@
         <v>80</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -1957,7 +1953,9 @@
       <c r="F27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="H27" s="1" t="s">
         <v>81</v>
       </c>
@@ -2334,7 +2332,7 @@
         <v>124</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>15</v>
@@ -2419,7 +2417,7 @@
         <v>80</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -2808,7 +2806,7 @@
         <v>176</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>15</v>
@@ -3024,7 +3022,7 @@
         <v>80</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H72" s="1"/>
     </row>
@@ -3656,7 +3654,7 @@
         <v>281</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>11</v>
@@ -3679,7 +3677,7 @@
         <v>284</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>15</v>
@@ -3714,7 +3712,7 @@
         <v>80</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing left-over debugging statement and updating module catalogue for MT4501 and MT4561
</commit_message>
<xml_diff>
--- a/module_catalogue/Module_catalogue.xlsx
+++ b/module_catalogue/Module_catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/Advising-tool/StA_Advising/module_catalogue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{8C6BC743-15A7-EA4C-86AF-11AAD9C0F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85D4F195-4770-B74A-84BB-2DA5C2EC65E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72EBC3-3DBF-D548-9FC8-658C17C7614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="49640" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="292">
   <si>
     <t>Module code</t>
   </si>
@@ -908,7 +908,10 @@
     <t>co-requisite MT4113 or MT5763</t>
   </si>
   <si>
-    <t>MT1007 or MT2508 or EC2203 or PH3012 and (MT3501 or MT3502 or MT3503 or MT3504 or MT3505 or MT3506 or MT3507 or MT3508)</t>
+    <t>co-requisite MT3501 or co-requisite MT3502 or co-requisite MT3503 or co-requisite MT3504 or co-requisite MT3505 or co-requisite MT3506 or co-requisite MT3507 or co-requisite MT3508</t>
+  </si>
+  <si>
+    <t>MT1007 or MT2508 or EC2203 or PH3012 and (co-requisite MT3501 or co-requisite MT3502 or co-requisite MT3503 or co-requisite MT3504 or co-requisite MT3505 or co-requisite MT3506 or co-requisite MT3507 or co-requisite MT3508)</t>
   </si>
 </sst>
 </file>
@@ -1294,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1957,7 @@
         <v>80</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>61</v>
+        <v>290</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>81</v>
@@ -3712,7 +3715,7 @@
         <v>80</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>